<commit_message>
add docs and data
</commit_message>
<xml_diff>
--- a/docs/Kich ban chuong trinh 2025.xlsx
+++ b/docs/Kich ban chuong trinh 2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KenIChi\Chatbot\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{48989525-4FFC-4973-B1AA-A0DEA66C4CC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA97B8E1-9A7F-44F9-9E9C-F6D8064E6226}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" firstSheet="1" activeTab="1" xr2:uid="{0FB9A36B-7D72-4241-814C-95ADC5B4EEAF}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" firstSheet="1" activeTab="7" xr2:uid="{0FB9A36B-7D72-4241-814C-95ADC5B4EEAF}"/>
   </bookViews>
   <sheets>
     <sheet name="Tổng thể kế hoạch tổ chức YEP" sheetId="6" r:id="rId1"/>
@@ -46,6 +46,7 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="7">'DS khách mời dự tính 2025'!$2:$2</definedName>
   </definedNames>
   <calcPr calcId="191028" concurrentManualCount="6"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -5993,18 +5994,18 @@
     <xf numFmtId="0" fontId="21" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -6023,6 +6024,15 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -6047,21 +6057,12 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -6080,6 +6081,42 @@
     <xf numFmtId="0" fontId="33" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="40" fillId="11" borderId="1" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="1" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="1" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="1" xfId="8" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="1" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="9" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="7" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="3" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="7" borderId="9" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="7" borderId="7" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="7" borderId="3" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="7" borderId="9" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="9" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -6113,42 +6150,6 @@
     <xf numFmtId="0" fontId="40" fillId="0" borderId="3" xfId="8" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="11" borderId="1" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="1" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="1" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="1" xfId="8" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="1" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="9" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="7" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="3" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="7" borderId="9" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="7" borderId="7" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="7" borderId="3" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="7" borderId="9" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -6185,6 +6186,48 @@
     <xf numFmtId="0" fontId="50" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="42" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="42" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="42" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="42" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="42" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="67" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -6194,50 +6237,8 @@
     <xf numFmtId="0" fontId="67" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="67" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="42" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="42" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="42" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="42" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="42" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -8351,19 +8352,19 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="409.5" customHeight="1">
-      <c r="A4" s="413">
+      <c r="A4" s="425">
         <v>1</v>
       </c>
-      <c r="B4" s="435" t="s">
+      <c r="B4" s="424" t="s">
         <v>161</v>
       </c>
-      <c r="C4" s="435" t="s">
+      <c r="C4" s="424" t="s">
         <v>162</v>
       </c>
-      <c r="D4" s="432" t="s">
+      <c r="D4" s="421" t="s">
         <v>163</v>
       </c>
-      <c r="E4" s="429" t="s">
+      <c r="E4" s="418" t="s">
         <v>164</v>
       </c>
       <c r="F4" s="233" t="s">
@@ -8374,51 +8375,51 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="115.15" hidden="1" customHeight="1">
-      <c r="A5" s="414"/>
-      <c r="B5" s="433"/>
-      <c r="C5" s="433"/>
-      <c r="D5" s="433"/>
-      <c r="E5" s="430"/>
+      <c r="A5" s="426"/>
+      <c r="B5" s="422"/>
+      <c r="C5" s="422"/>
+      <c r="D5" s="422"/>
+      <c r="E5" s="419"/>
       <c r="F5" s="233"/>
     </row>
     <row r="6" spans="1:7" ht="129" hidden="1" customHeight="1">
-      <c r="A6" s="414"/>
-      <c r="B6" s="433"/>
-      <c r="C6" s="433"/>
-      <c r="D6" s="433"/>
-      <c r="E6" s="430"/>
+      <c r="A6" s="426"/>
+      <c r="B6" s="422"/>
+      <c r="C6" s="422"/>
+      <c r="D6" s="422"/>
+      <c r="E6" s="419"/>
       <c r="F6" s="233"/>
     </row>
     <row r="7" spans="1:7" ht="118.15" hidden="1" customHeight="1">
-      <c r="A7" s="414"/>
-      <c r="B7" s="433"/>
-      <c r="C7" s="433"/>
-      <c r="D7" s="433"/>
-      <c r="E7" s="430"/>
+      <c r="A7" s="426"/>
+      <c r="B7" s="422"/>
+      <c r="C7" s="422"/>
+      <c r="D7" s="422"/>
+      <c r="E7" s="419"/>
       <c r="F7" s="233"/>
     </row>
     <row r="8" spans="1:7" ht="175.5" customHeight="1">
-      <c r="A8" s="415"/>
-      <c r="B8" s="434"/>
-      <c r="C8" s="434"/>
-      <c r="D8" s="434"/>
-      <c r="E8" s="431"/>
+      <c r="A8" s="427"/>
+      <c r="B8" s="423"/>
+      <c r="C8" s="423"/>
+      <c r="D8" s="423"/>
+      <c r="E8" s="420"/>
       <c r="F8" s="233"/>
     </row>
     <row r="9" spans="1:7" ht="409.5" customHeight="1">
       <c r="A9" s="219" t="s">
         <v>167</v>
       </c>
-      <c r="B9" s="416" t="s">
+      <c r="B9" s="428" t="s">
         <v>168</v>
       </c>
-      <c r="C9" s="418" t="s">
+      <c r="C9" s="430" t="s">
         <v>169</v>
       </c>
-      <c r="D9" s="420" t="s">
+      <c r="D9" s="432" t="s">
         <v>170</v>
       </c>
-      <c r="E9" s="422" t="s">
+      <c r="E9" s="434" t="s">
         <v>171</v>
       </c>
       <c r="F9" s="235"/>
@@ -8428,10 +8429,10 @@
     </row>
     <row r="10" spans="1:7" ht="147" customHeight="1">
       <c r="A10" s="219"/>
-      <c r="B10" s="417"/>
-      <c r="C10" s="419"/>
-      <c r="D10" s="421"/>
-      <c r="E10" s="423"/>
+      <c r="B10" s="429"/>
+      <c r="C10" s="431"/>
+      <c r="D10" s="433"/>
+      <c r="E10" s="435"/>
       <c r="F10" s="235"/>
       <c r="G10" s="205"/>
     </row>
@@ -8439,16 +8440,16 @@
       <c r="A11" s="221">
         <v>7</v>
       </c>
-      <c r="B11" s="426" t="s">
+      <c r="B11" s="415" t="s">
         <v>173</v>
       </c>
-      <c r="C11" s="425" t="s">
+      <c r="C11" s="414" t="s">
         <v>174</v>
       </c>
-      <c r="D11" s="424" t="s">
+      <c r="D11" s="413" t="s">
         <v>175</v>
       </c>
-      <c r="E11" s="427" t="s">
+      <c r="E11" s="416" t="s">
         <v>176</v>
       </c>
       <c r="F11" s="234" t="s">
@@ -8460,15 +8461,20 @@
     </row>
     <row r="12" spans="1:7" ht="103.5" customHeight="1">
       <c r="A12" s="220"/>
-      <c r="B12" s="426"/>
-      <c r="C12" s="425"/>
-      <c r="D12" s="424"/>
-      <c r="E12" s="428"/>
+      <c r="B12" s="415"/>
+      <c r="C12" s="414"/>
+      <c r="D12" s="413"/>
+      <c r="E12" s="417"/>
       <c r="F12" s="234"/>
       <c r="G12" s="296"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A4:A8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
     <mergeCell ref="D11:D12"/>
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="B11:B12"/>
@@ -8477,11 +8483,6 @@
     <mergeCell ref="D4:D8"/>
     <mergeCell ref="C4:C8"/>
     <mergeCell ref="B4:B8"/>
-    <mergeCell ref="A4:A8"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
   </mergeCells>
   <pageMargins left="0.31496062992125984" right="0.31496062992125984" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="44" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -8517,21 +8518,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="30.75" customHeight="1">
-      <c r="A1" s="400" t="s">
+      <c r="A1" s="403" t="s">
         <v>179</v>
       </c>
-      <c r="B1" s="400"/>
-      <c r="C1" s="400"/>
-      <c r="D1" s="400"/>
-      <c r="E1" s="400"/>
-      <c r="F1" s="400"/>
-      <c r="G1" s="400"/>
+      <c r="B1" s="403"/>
+      <c r="C1" s="403"/>
+      <c r="D1" s="403"/>
+      <c r="E1" s="403"/>
+      <c r="F1" s="403"/>
+      <c r="G1" s="403"/>
     </row>
     <row r="2" spans="1:12">
-      <c r="A2" s="401" t="s">
+      <c r="A2" s="404" t="s">
         <v>180</v>
       </c>
-      <c r="B2" s="401"/>
+      <c r="B2" s="404"/>
       <c r="C2" s="182"/>
       <c r="D2" s="63"/>
       <c r="E2" s="183"/>
@@ -8562,7 +8563,7 @@
       <c r="G3" s="64"/>
     </row>
     <row r="4" spans="1:12" ht="44.25" customHeight="1">
-      <c r="A4" s="402" t="s">
+      <c r="A4" s="394" t="s">
         <v>188</v>
       </c>
       <c r="B4" s="66" t="s">
@@ -8581,14 +8582,14 @@
       <c r="F4" s="436" t="s">
         <v>190</v>
       </c>
-      <c r="G4" s="404"/>
+      <c r="G4" s="405"/>
       <c r="I4"/>
       <c r="J4"/>
       <c r="K4"/>
       <c r="L4"/>
     </row>
     <row r="5" spans="1:12" ht="44.25" customHeight="1">
-      <c r="A5" s="403"/>
+      <c r="A5" s="395"/>
       <c r="B5" s="68" t="s">
         <v>191</v>
       </c>
@@ -8602,7 +8603,7 @@
         <v>2000</v>
       </c>
       <c r="F5" s="436"/>
-      <c r="G5" s="405"/>
+      <c r="G5" s="406"/>
       <c r="I5"/>
       <c r="J5"/>
       <c r="K5">
@@ -8611,7 +8612,7 @@
       <c r="L5"/>
     </row>
     <row r="6" spans="1:12" ht="66" customHeight="1">
-      <c r="A6" s="403"/>
+      <c r="A6" s="395"/>
       <c r="B6" s="280" t="s">
         <v>192</v>
       </c>
@@ -8624,15 +8625,15 @@
       <c r="E6" s="193">
         <v>4680</v>
       </c>
-      <c r="F6" s="405"/>
-      <c r="G6" s="405"/>
+      <c r="F6" s="406"/>
+      <c r="G6" s="406"/>
       <c r="I6"/>
       <c r="J6"/>
       <c r="K6"/>
       <c r="L6"/>
     </row>
     <row r="7" spans="1:12" ht="66" customHeight="1">
-      <c r="A7" s="403"/>
+      <c r="A7" s="395"/>
       <c r="B7" s="70" t="s">
         <v>193</v>
       </c>
@@ -8645,15 +8646,15 @@
       <c r="E7" s="186">
         <v>340</v>
       </c>
-      <c r="F7" s="405"/>
-      <c r="G7" s="405"/>
+      <c r="F7" s="406"/>
+      <c r="G7" s="406"/>
       <c r="I7"/>
       <c r="J7"/>
       <c r="K7"/>
       <c r="L7"/>
     </row>
     <row r="8" spans="1:12" ht="57" customHeight="1">
-      <c r="A8" s="403"/>
+      <c r="A8" s="395"/>
       <c r="B8" s="70" t="s">
         <v>194</v>
       </c>
@@ -8667,14 +8668,14 @@
         <v>180</v>
       </c>
       <c r="F8" s="437"/>
-      <c r="G8" s="405"/>
+      <c r="G8" s="406"/>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8"/>
       <c r="L8"/>
     </row>
     <row r="9" spans="1:12" ht="33" customHeight="1">
-      <c r="A9" s="402" t="s">
+      <c r="A9" s="394" t="s">
         <v>195</v>
       </c>
       <c r="B9" s="189" t="s">
@@ -8699,7 +8700,7 @@
       <c r="L9"/>
     </row>
     <row r="10" spans="1:12" ht="33" customHeight="1">
-      <c r="A10" s="403"/>
+      <c r="A10" s="395"/>
       <c r="B10" s="189" t="s">
         <v>197</v>
       </c>
@@ -8720,7 +8721,7 @@
       <c r="L10"/>
     </row>
     <row r="11" spans="1:12" ht="33" customHeight="1">
-      <c r="A11" s="406"/>
+      <c r="A11" s="396"/>
       <c r="B11" s="294" t="s">
         <v>198</v>
       </c>
@@ -8784,7 +8785,7 @@
       <c r="G13" s="41"/>
     </row>
     <row r="14" spans="1:12" ht="14.5">
-      <c r="A14" s="394" t="s">
+      <c r="A14" s="397" t="s">
         <v>204</v>
       </c>
       <c r="B14" s="286" t="s">
@@ -8805,7 +8806,7 @@
       <c r="L14"/>
     </row>
     <row r="15" spans="1:12" ht="14.5">
-      <c r="A15" s="395"/>
+      <c r="A15" s="398"/>
       <c r="B15" s="289" t="s">
         <v>206</v>
       </c>
@@ -8825,7 +8826,7 @@
       <c r="L15"/>
     </row>
     <row r="16" spans="1:12" ht="14.5">
-      <c r="A16" s="395"/>
+      <c r="A16" s="398"/>
       <c r="B16" s="289" t="s">
         <v>207</v>
       </c>
@@ -8845,7 +8846,7 @@
       <c r="L16"/>
     </row>
     <row r="17" spans="1:12" ht="14.5">
-      <c r="A17" s="395"/>
+      <c r="A17" s="398"/>
       <c r="B17" s="289" t="s">
         <v>208</v>
       </c>
@@ -8866,7 +8867,7 @@
       <c r="L17"/>
     </row>
     <row r="18" spans="1:12" ht="14.5">
-      <c r="A18" s="395"/>
+      <c r="A18" s="398"/>
       <c r="B18" s="293" t="s">
         <v>209</v>
       </c>
@@ -8886,7 +8887,7 @@
       <c r="L18"/>
     </row>
     <row r="19" spans="1:12" ht="31.5" customHeight="1">
-      <c r="A19" s="395"/>
+      <c r="A19" s="398"/>
       <c r="B19" s="195" t="s">
         <v>210</v>
       </c>
@@ -8909,7 +8910,7 @@
       <c r="L19"/>
     </row>
     <row r="20" spans="1:12" ht="175.5" customHeight="1">
-      <c r="A20" s="396"/>
+      <c r="A20" s="399"/>
       <c r="B20" s="70" t="s">
         <v>212</v>
       </c>
@@ -8949,12 +8950,12 @@
       <c r="L21"/>
     </row>
     <row r="22" spans="1:12" ht="27" customHeight="1">
-      <c r="A22" s="397" t="s">
+      <c r="A22" s="400" t="s">
         <v>215</v>
       </c>
-      <c r="B22" s="398"/>
-      <c r="C22" s="398"/>
-      <c r="D22" s="399"/>
+      <c r="B22" s="401"/>
+      <c r="C22" s="401"/>
+      <c r="D22" s="402"/>
       <c r="E22" s="196">
         <f>SUM(E4:E21)</f>
         <v>50895</v>
@@ -8966,12 +8967,12 @@
       <c r="L22"/>
     </row>
     <row r="23" spans="1:12" ht="27" customHeight="1">
-      <c r="A23" s="397" t="s">
+      <c r="A23" s="400" t="s">
         <v>216</v>
       </c>
-      <c r="B23" s="398"/>
-      <c r="C23" s="398"/>
-      <c r="D23" s="399"/>
+      <c r="B23" s="401"/>
+      <c r="C23" s="401"/>
+      <c r="D23" s="402"/>
       <c r="E23" s="196">
         <f>'DS khách mời dự tính 2024'!H79</f>
         <v>51300</v>
@@ -11663,13 +11664,13 @@
     </row>
     <row r="6" spans="1:9" ht="409.6" customHeight="1">
       <c r="A6" s="412"/>
-      <c r="B6" s="460" t="s">
+      <c r="B6" s="451" t="s">
         <v>427</v>
       </c>
-      <c r="C6" s="451" t="s">
+      <c r="C6" s="460" t="s">
         <v>127</v>
       </c>
-      <c r="D6" s="451" t="s">
+      <c r="D6" s="460" t="s">
         <v>378</v>
       </c>
       <c r="E6" s="457"/>
@@ -11678,60 +11679,60 @@
         <v>428</v>
       </c>
       <c r="H6" s="100"/>
-      <c r="I6" s="448" t="s">
+      <c r="I6" s="462" t="s">
         <v>429</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="340.5" customHeight="1">
       <c r="A7" s="266"/>
-      <c r="B7" s="461"/>
-      <c r="C7" s="452"/>
-      <c r="D7" s="452"/>
+      <c r="B7" s="452"/>
+      <c r="C7" s="461"/>
+      <c r="D7" s="461"/>
       <c r="E7" s="457"/>
       <c r="F7" s="102"/>
       <c r="G7" s="99"/>
       <c r="H7" s="100"/>
-      <c r="I7" s="448"/>
+      <c r="I7" s="462"/>
     </row>
     <row r="8" spans="1:9" ht="409.6" customHeight="1">
       <c r="A8" s="412"/>
-      <c r="B8" s="460" t="s">
+      <c r="B8" s="451" t="s">
         <v>430</v>
       </c>
-      <c r="C8" s="454" t="s">
+      <c r="C8" s="449" t="s">
         <v>123</v>
       </c>
-      <c r="D8" s="451" t="s">
+      <c r="D8" s="460" t="s">
         <v>431</v>
       </c>
       <c r="E8" s="457"/>
       <c r="F8" s="102"/>
       <c r="G8" s="99"/>
       <c r="H8" s="100"/>
-      <c r="I8" s="449" t="s">
+      <c r="I8" s="463" t="s">
         <v>432</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="38.25" customHeight="1">
       <c r="A9" s="412"/>
-      <c r="B9" s="461"/>
-      <c r="C9" s="456"/>
-      <c r="D9" s="452"/>
+      <c r="B9" s="452"/>
+      <c r="C9" s="450"/>
+      <c r="D9" s="461"/>
       <c r="E9" s="101"/>
       <c r="F9" s="102"/>
       <c r="G9" s="99"/>
       <c r="H9" s="100"/>
-      <c r="I9" s="450"/>
+      <c r="I9" s="464"/>
     </row>
     <row r="10" spans="1:9" ht="358.9" customHeight="1">
       <c r="A10" s="412"/>
-      <c r="B10" s="463" t="s">
+      <c r="B10" s="453" t="s">
         <v>433</v>
       </c>
-      <c r="C10" s="454" t="s">
+      <c r="C10" s="449" t="s">
         <v>130</v>
       </c>
-      <c r="D10" s="454" t="s">
+      <c r="D10" s="449" t="s">
         <v>434</v>
       </c>
       <c r="E10" s="101" t="s">
@@ -11744,31 +11745,31 @@
         <v>436</v>
       </c>
       <c r="H10" s="100"/>
-      <c r="I10" s="449" t="s">
+      <c r="I10" s="463" t="s">
         <v>437</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="409.15" customHeight="1">
       <c r="A11" s="412"/>
-      <c r="B11" s="464"/>
-      <c r="C11" s="455"/>
-      <c r="D11" s="455"/>
+      <c r="B11" s="454"/>
+      <c r="C11" s="456"/>
+      <c r="D11" s="456"/>
       <c r="E11" s="237"/>
       <c r="F11" s="98"/>
       <c r="G11" s="99"/>
       <c r="H11" s="100"/>
-      <c r="I11" s="453"/>
+      <c r="I11" s="465"/>
     </row>
     <row r="12" spans="1:9" ht="42.65" customHeight="1">
       <c r="A12" s="412"/>
-      <c r="B12" s="465"/>
-      <c r="C12" s="456"/>
-      <c r="D12" s="456"/>
+      <c r="B12" s="455"/>
+      <c r="C12" s="450"/>
+      <c r="D12" s="450"/>
       <c r="E12" s="237"/>
       <c r="F12" s="98"/>
       <c r="G12" s="99"/>
       <c r="H12" s="100"/>
-      <c r="I12" s="450"/>
+      <c r="I12" s="464"/>
     </row>
     <row r="13" spans="1:9" ht="117.75" customHeight="1">
       <c r="A13" s="412"/>
@@ -11813,7 +11814,7 @@
       <c r="G14" s="99" t="s">
         <v>444</v>
       </c>
-      <c r="H14" s="462" t="s">
+      <c r="H14" s="448" t="s">
         <v>445</v>
       </c>
       <c r="I14" s="274" t="s">
@@ -11836,7 +11837,7 @@
       <c r="G15" s="99" t="s">
         <v>449</v>
       </c>
-      <c r="H15" s="462"/>
+      <c r="H15" s="448"/>
       <c r="I15" s="275" t="s">
         <v>397</v>
       </c>
@@ -11857,7 +11858,7 @@
       <c r="G16" s="99" t="s">
         <v>451</v>
       </c>
-      <c r="H16" s="462"/>
+      <c r="H16" s="448"/>
       <c r="I16" s="275" t="s">
         <v>399</v>
       </c>
@@ -11880,7 +11881,7 @@
       <c r="G17" s="99" t="s">
         <v>454</v>
       </c>
-      <c r="H17" s="462"/>
+      <c r="H17" s="448"/>
       <c r="I17" s="275" t="s">
         <v>402</v>
       </c>
@@ -11929,6 +11930,18 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="I10:I12"/>
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="E4:E8"/>
+    <mergeCell ref="A10:A19"/>
+    <mergeCell ref="E13:E17"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="B6:B7"/>
     <mergeCell ref="H14:H17"/>
     <mergeCell ref="E18:E19"/>
     <mergeCell ref="C8:C9"/>
@@ -11936,18 +11949,6 @@
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="B10:B12"/>
     <mergeCell ref="C10:C12"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="E4:E8"/>
-    <mergeCell ref="A10:A19"/>
-    <mergeCell ref="E13:E17"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="I10:I12"/>
-    <mergeCell ref="D10:D12"/>
   </mergeCells>
   <pageMargins left="0.27559055118110237" right="0.15748031496062992" top="0.39370078740157483" bottom="0.27559055118110237" header="0.47244094488188981" footer="0.23622047244094491"/>
   <pageSetup paperSize="11" scale="22" orientation="portrait" r:id="rId1"/>
@@ -12499,10 +12500,10 @@
       <c r="G1" s="475"/>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="401" t="s">
+      <c r="A2" s="404" t="s">
         <v>180</v>
       </c>
-      <c r="B2" s="401"/>
+      <c r="B2" s="404"/>
       <c r="C2" s="34"/>
       <c r="D2" s="63"/>
       <c r="E2" s="476" t="s">
@@ -12535,7 +12536,7 @@
       <c r="G3" s="64"/>
     </row>
     <row r="4" spans="1:11" ht="33" customHeight="1">
-      <c r="A4" s="402" t="s">
+      <c r="A4" s="394" t="s">
         <v>512</v>
       </c>
       <c r="B4" s="66" t="s">
@@ -12551,14 +12552,14 @@
         <f>C4*D4</f>
         <v>24560000</v>
       </c>
-      <c r="F4" s="404"/>
-      <c r="G4" s="404"/>
+      <c r="F4" s="405"/>
+      <c r="G4" s="405"/>
       <c r="I4"/>
       <c r="J4"/>
       <c r="K4"/>
     </row>
     <row r="5" spans="1:11" ht="33" customHeight="1">
-      <c r="A5" s="403"/>
+      <c r="A5" s="395"/>
       <c r="B5" s="68" t="s">
         <v>514</v>
       </c>
@@ -12571,14 +12572,14 @@
       <c r="E5" s="38">
         <v>4581000</v>
       </c>
-      <c r="F5" s="405"/>
-      <c r="G5" s="405"/>
+      <c r="F5" s="406"/>
+      <c r="G5" s="406"/>
       <c r="I5"/>
       <c r="J5"/>
       <c r="K5"/>
     </row>
     <row r="6" spans="1:11" ht="33" customHeight="1">
-      <c r="A6" s="403"/>
+      <c r="A6" s="395"/>
       <c r="B6" s="70" t="s">
         <v>516</v>
       </c>
@@ -12591,14 +12592,14 @@
       <c r="E6" s="39">
         <v>398000</v>
       </c>
-      <c r="F6" s="405"/>
-      <c r="G6" s="405"/>
+      <c r="F6" s="406"/>
+      <c r="G6" s="406"/>
       <c r="I6"/>
       <c r="J6"/>
       <c r="K6"/>
     </row>
     <row r="7" spans="1:11" ht="33" customHeight="1">
-      <c r="A7" s="403"/>
+      <c r="A7" s="395"/>
       <c r="B7" s="70" t="s">
         <v>518</v>
       </c>
@@ -12611,14 +12612,14 @@
       <c r="E7" s="39">
         <v>233000</v>
       </c>
-      <c r="F7" s="405"/>
-      <c r="G7" s="405"/>
+      <c r="F7" s="406"/>
+      <c r="G7" s="406"/>
       <c r="I7"/>
       <c r="J7"/>
       <c r="K7"/>
     </row>
     <row r="8" spans="1:11" ht="33" customHeight="1">
-      <c r="A8" s="403"/>
+      <c r="A8" s="395"/>
       <c r="B8" s="70" t="s">
         <v>520</v>
       </c>
@@ -12631,14 +12632,14 @@
       <c r="E8" s="39">
         <v>1500000</v>
       </c>
-      <c r="F8" s="405"/>
-      <c r="G8" s="405"/>
+      <c r="F8" s="406"/>
+      <c r="G8" s="406"/>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8"/>
     </row>
     <row r="9" spans="1:11" ht="33" customHeight="1">
-      <c r="A9" s="406"/>
+      <c r="A9" s="396"/>
       <c r="B9" s="72" t="s">
         <v>521</v>
       </c>
@@ -12678,7 +12679,7 @@
       </c>
     </row>
     <row r="11" spans="1:11" ht="30.75" customHeight="1">
-      <c r="A11" s="394" t="s">
+      <c r="A11" s="397" t="s">
         <v>527</v>
       </c>
       <c r="B11" s="76" t="s">
@@ -12699,7 +12700,7 @@
       <c r="G11" s="41"/>
     </row>
     <row r="12" spans="1:11" ht="27" customHeight="1">
-      <c r="A12" s="395"/>
+      <c r="A12" s="398"/>
       <c r="B12" s="78" t="s">
         <v>530</v>
       </c>
@@ -12715,7 +12716,7 @@
       <c r="G12" s="43"/>
     </row>
     <row r="13" spans="1:11" ht="18.75" customHeight="1">
-      <c r="A13" s="396"/>
+      <c r="A13" s="399"/>
       <c r="B13" s="68" t="s">
         <v>532</v>
       </c>
@@ -12753,7 +12754,7 @@
       <c r="G14" s="45"/>
     </row>
     <row r="15" spans="1:11" ht="42">
-      <c r="A15" s="395" t="s">
+      <c r="A15" s="398" t="s">
         <v>536</v>
       </c>
       <c r="B15" s="87" t="s">
@@ -12772,7 +12773,7 @@
       <c r="G15" s="43"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="396"/>
+      <c r="A16" s="399"/>
       <c r="B16" s="89" t="s">
         <v>540</v>
       </c>
@@ -12809,12 +12810,12 @@
       </c>
     </row>
     <row r="18" spans="1:7" ht="27" customHeight="1">
-      <c r="A18" s="397" t="s">
+      <c r="A18" s="400" t="s">
         <v>546</v>
       </c>
-      <c r="B18" s="398"/>
-      <c r="C18" s="398"/>
-      <c r="D18" s="399"/>
+      <c r="B18" s="401"/>
+      <c r="C18" s="401"/>
+      <c r="D18" s="402"/>
       <c r="E18" s="46">
         <f>SUM(E4:E17)</f>
         <v>43440000</v>
@@ -12823,12 +12824,12 @@
       <c r="G18" s="48"/>
     </row>
     <row r="19" spans="1:7" ht="27" customHeight="1">
-      <c r="A19" s="397" t="s">
+      <c r="A19" s="400" t="s">
         <v>547</v>
       </c>
-      <c r="B19" s="398"/>
-      <c r="C19" s="398"/>
-      <c r="D19" s="399"/>
+      <c r="B19" s="401"/>
+      <c r="C19" s="401"/>
+      <c r="D19" s="402"/>
       <c r="E19" s="46">
         <v>45750000</v>
       </c>
@@ -12836,12 +12837,12 @@
       <c r="G19" s="48"/>
     </row>
     <row r="20" spans="1:7" ht="27" customHeight="1">
-      <c r="A20" s="397" t="s">
+      <c r="A20" s="400" t="s">
         <v>548</v>
       </c>
-      <c r="B20" s="398"/>
-      <c r="C20" s="398"/>
-      <c r="D20" s="399"/>
+      <c r="B20" s="401"/>
+      <c r="C20" s="401"/>
+      <c r="D20" s="402"/>
       <c r="E20" s="49">
         <v>2220000</v>
       </c>
@@ -12886,8 +12887,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2ACF419-3E08-40BF-B3CA-E977B45AA147}">
   <dimension ref="B2:J52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14"/>
@@ -13616,140 +13617,140 @@
     <row r="21" spans="1:8" ht="35.25" customHeight="1">
       <c r="A21" s="377"/>
       <c r="B21" s="31"/>
-      <c r="C21" s="385"/>
-      <c r="D21" s="385"/>
-      <c r="E21" s="385"/>
-      <c r="F21" s="385"/>
-      <c r="G21" s="385"/>
+      <c r="C21" s="387"/>
+      <c r="D21" s="387"/>
+      <c r="E21" s="387"/>
+      <c r="F21" s="387"/>
+      <c r="G21" s="387"/>
     </row>
     <row r="22" spans="1:8" s="32" customFormat="1">
       <c r="A22" s="377"/>
-      <c r="B22" s="386"/>
-      <c r="C22" s="387"/>
-      <c r="D22" s="387"/>
-      <c r="E22" s="387"/>
-      <c r="F22" s="387"/>
-      <c r="G22" s="387"/>
+      <c r="B22" s="384"/>
+      <c r="C22" s="385"/>
+      <c r="D22" s="385"/>
+      <c r="E22" s="385"/>
+      <c r="F22" s="385"/>
+      <c r="G22" s="385"/>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="377"/>
-      <c r="B23" s="386"/>
-      <c r="C23" s="387"/>
-      <c r="D23" s="387"/>
-      <c r="E23" s="387"/>
-      <c r="F23" s="387"/>
-      <c r="G23" s="387"/>
+      <c r="B23" s="384"/>
+      <c r="C23" s="385"/>
+      <c r="D23" s="385"/>
+      <c r="E23" s="385"/>
+      <c r="F23" s="385"/>
+      <c r="G23" s="385"/>
       <c r="H23" s="12" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="377"/>
-      <c r="B24" s="386"/>
-      <c r="C24" s="387"/>
-      <c r="D24" s="387"/>
-      <c r="E24" s="387"/>
-      <c r="F24" s="387"/>
-      <c r="G24" s="387"/>
+      <c r="B24" s="384"/>
+      <c r="C24" s="385"/>
+      <c r="D24" s="385"/>
+      <c r="E24" s="385"/>
+      <c r="F24" s="385"/>
+      <c r="G24" s="385"/>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="377"/>
-      <c r="B25" s="386"/>
-      <c r="C25" s="387"/>
-      <c r="D25" s="387"/>
-      <c r="E25" s="387"/>
-      <c r="F25" s="387"/>
-      <c r="G25" s="387"/>
+      <c r="B25" s="384"/>
+      <c r="C25" s="385"/>
+      <c r="D25" s="385"/>
+      <c r="E25" s="385"/>
+      <c r="F25" s="385"/>
+      <c r="G25" s="385"/>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="377"/>
-      <c r="B26" s="386"/>
-      <c r="C26" s="387"/>
-      <c r="D26" s="387"/>
-      <c r="E26" s="387"/>
-      <c r="F26" s="387"/>
-      <c r="G26" s="387"/>
+      <c r="B26" s="384"/>
+      <c r="C26" s="385"/>
+      <c r="D26" s="385"/>
+      <c r="E26" s="385"/>
+      <c r="F26" s="385"/>
+      <c r="G26" s="385"/>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="377"/>
-      <c r="B27" s="386"/>
-      <c r="C27" s="387"/>
-      <c r="D27" s="387"/>
-      <c r="E27" s="387"/>
-      <c r="F27" s="387"/>
-      <c r="G27" s="387"/>
+      <c r="B27" s="384"/>
+      <c r="C27" s="385"/>
+      <c r="D27" s="385"/>
+      <c r="E27" s="385"/>
+      <c r="F27" s="385"/>
+      <c r="G27" s="385"/>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="377"/>
-      <c r="B28" s="386"/>
-      <c r="C28" s="387"/>
-      <c r="D28" s="387"/>
-      <c r="E28" s="387"/>
-      <c r="F28" s="387"/>
-      <c r="G28" s="387"/>
+      <c r="B28" s="384"/>
+      <c r="C28" s="385"/>
+      <c r="D28" s="385"/>
+      <c r="E28" s="385"/>
+      <c r="F28" s="385"/>
+      <c r="G28" s="385"/>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="377"/>
-      <c r="B29" s="386"/>
-      <c r="C29" s="387"/>
-      <c r="D29" s="387"/>
-      <c r="E29" s="387"/>
-      <c r="F29" s="387"/>
-      <c r="G29" s="387"/>
+      <c r="B29" s="384"/>
+      <c r="C29" s="385"/>
+      <c r="D29" s="385"/>
+      <c r="E29" s="385"/>
+      <c r="F29" s="385"/>
+      <c r="G29" s="385"/>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="377"/>
-      <c r="B30" s="386"/>
-      <c r="C30" s="387"/>
-      <c r="D30" s="387"/>
-      <c r="E30" s="387"/>
-      <c r="F30" s="387"/>
-      <c r="G30" s="387"/>
+      <c r="B30" s="384"/>
+      <c r="C30" s="385"/>
+      <c r="D30" s="385"/>
+      <c r="E30" s="385"/>
+      <c r="F30" s="385"/>
+      <c r="G30" s="385"/>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="377"/>
-      <c r="B31" s="386"/>
-      <c r="C31" s="387"/>
-      <c r="D31" s="387"/>
-      <c r="E31" s="387"/>
-      <c r="F31" s="387"/>
-      <c r="G31" s="387"/>
+      <c r="B31" s="384"/>
+      <c r="C31" s="385"/>
+      <c r="D31" s="385"/>
+      <c r="E31" s="385"/>
+      <c r="F31" s="385"/>
+      <c r="G31" s="385"/>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="377"/>
-      <c r="B32" s="386"/>
-      <c r="C32" s="387"/>
-      <c r="D32" s="387"/>
-      <c r="E32" s="387"/>
-      <c r="F32" s="387"/>
-      <c r="G32" s="387"/>
+      <c r="B32" s="384"/>
+      <c r="C32" s="385"/>
+      <c r="D32" s="385"/>
+      <c r="E32" s="385"/>
+      <c r="F32" s="385"/>
+      <c r="G32" s="385"/>
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="377"/>
-      <c r="B33" s="386"/>
-      <c r="C33" s="387"/>
-      <c r="D33" s="387"/>
-      <c r="E33" s="387"/>
-      <c r="F33" s="387"/>
-      <c r="G33" s="387"/>
+      <c r="B33" s="384"/>
+      <c r="C33" s="385"/>
+      <c r="D33" s="385"/>
+      <c r="E33" s="385"/>
+      <c r="F33" s="385"/>
+      <c r="G33" s="385"/>
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="377"/>
-      <c r="B34" s="386"/>
-      <c r="C34" s="387"/>
-      <c r="D34" s="387"/>
-      <c r="E34" s="387"/>
-      <c r="F34" s="387"/>
-      <c r="G34" s="387"/>
+      <c r="B34" s="384"/>
+      <c r="C34" s="385"/>
+      <c r="D34" s="385"/>
+      <c r="E34" s="385"/>
+      <c r="F34" s="385"/>
+      <c r="G34" s="385"/>
     </row>
     <row r="35" spans="1:7">
       <c r="A35" s="377"/>
-      <c r="B35" s="386"/>
-      <c r="C35" s="387"/>
-      <c r="D35" s="387"/>
-      <c r="E35" s="387"/>
-      <c r="F35" s="387"/>
-      <c r="G35" s="387"/>
+      <c r="B35" s="384"/>
+      <c r="C35" s="385"/>
+      <c r="D35" s="385"/>
+      <c r="E35" s="385"/>
+      <c r="F35" s="385"/>
+      <c r="G35" s="385"/>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="377"/>
@@ -13780,11 +13781,13 @@
       <c r="B42" s="14"/>
     </row>
     <row r="43" spans="1:7">
-      <c r="A43" s="384"/>
+      <c r="A43" s="386"/>
       <c r="B43" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B30:G30"/>
+    <mergeCell ref="B31:G31"/>
     <mergeCell ref="B32:G32"/>
     <mergeCell ref="B33:G33"/>
     <mergeCell ref="A1:G1"/>
@@ -13801,8 +13804,6 @@
     <mergeCell ref="B35:G35"/>
     <mergeCell ref="B28:G28"/>
     <mergeCell ref="B29:G29"/>
-    <mergeCell ref="B30:G30"/>
-    <mergeCell ref="B31:G31"/>
   </mergeCells>
   <phoneticPr fontId="6"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -14517,7 +14518,7 @@
   <dimension ref="A1:M25"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" topLeftCell="A4" zoomScale="70" zoomScaleNormal="85" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -14539,22 +14540,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="30.75" customHeight="1">
-      <c r="A1" s="400" t="s">
+      <c r="A1" s="403" t="s">
         <v>179</v>
       </c>
-      <c r="B1" s="400"/>
-      <c r="C1" s="400"/>
-      <c r="D1" s="400"/>
-      <c r="E1" s="400"/>
-      <c r="F1" s="400"/>
-      <c r="G1" s="400"/>
+      <c r="B1" s="403"/>
+      <c r="C1" s="403"/>
+      <c r="D1" s="403"/>
+      <c r="E1" s="403"/>
+      <c r="F1" s="403"/>
+      <c r="G1" s="403"/>
       <c r="H1" s="368"/>
     </row>
     <row r="2" spans="1:13">
-      <c r="A2" s="401" t="s">
+      <c r="A2" s="404" t="s">
         <v>180</v>
       </c>
-      <c r="B2" s="401"/>
+      <c r="B2" s="404"/>
       <c r="C2" s="182"/>
       <c r="D2" s="322"/>
       <c r="E2" s="183"/>
@@ -14587,7 +14588,7 @@
       <c r="H3" s="371"/>
     </row>
     <row r="4" spans="1:13" ht="44.25" customHeight="1">
-      <c r="A4" s="402" t="s">
+      <c r="A4" s="394" t="s">
         <v>188</v>
       </c>
       <c r="B4" s="351" t="s">
@@ -14603,10 +14604,10 @@
         <f>C4*D4</f>
         <v>31600</v>
       </c>
-      <c r="F4" s="404"/>
-      <c r="G4" s="404"/>
+      <c r="F4" s="405"/>
+      <c r="G4" s="405"/>
       <c r="H4" s="345"/>
-      <c r="I4" s="402" t="s">
+      <c r="I4" s="394" t="s">
         <v>188</v>
       </c>
       <c r="J4" s="66" t="s">
@@ -14624,7 +14625,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" ht="44.25" customHeight="1">
-      <c r="A5" s="403"/>
+      <c r="A5" s="395"/>
       <c r="B5" s="354" t="s">
         <v>583</v>
       </c>
@@ -14638,10 +14639,10 @@
         <f t="shared" ref="E5" si="0">C5*D5</f>
         <v>5000</v>
       </c>
-      <c r="F5" s="405"/>
-      <c r="G5" s="405"/>
+      <c r="F5" s="406"/>
+      <c r="G5" s="406"/>
       <c r="H5" s="346"/>
-      <c r="I5" s="403"/>
+      <c r="I5" s="395"/>
       <c r="J5" s="68" t="s">
         <v>191</v>
       </c>
@@ -14656,7 +14657,7 @@
       </c>
     </row>
     <row r="6" spans="1:13" ht="44.25" customHeight="1">
-      <c r="A6" s="403"/>
+      <c r="A6" s="395"/>
       <c r="B6" s="354" t="s">
         <v>582</v>
       </c>
@@ -14670,10 +14671,10 @@
         <f t="shared" ref="E6:E19" si="1">C6*D6</f>
         <v>3000</v>
       </c>
-      <c r="F6" s="405"/>
-      <c r="G6" s="405"/>
+      <c r="F6" s="406"/>
+      <c r="G6" s="406"/>
       <c r="H6" s="346"/>
-      <c r="I6" s="403"/>
+      <c r="I6" s="395"/>
       <c r="J6" s="280" t="s">
         <v>192</v>
       </c>
@@ -14688,7 +14689,7 @@
       </c>
     </row>
     <row r="7" spans="1:13" ht="66" customHeight="1">
-      <c r="A7" s="403"/>
+      <c r="A7" s="395"/>
       <c r="B7" s="280" t="s">
         <v>581</v>
       </c>
@@ -14702,10 +14703,10 @@
         <f t="shared" si="1"/>
         <v>5400</v>
       </c>
-      <c r="F7" s="405"/>
-      <c r="G7" s="405"/>
+      <c r="F7" s="406"/>
+      <c r="G7" s="406"/>
       <c r="H7" s="346"/>
-      <c r="I7" s="403"/>
+      <c r="I7" s="395"/>
       <c r="J7" s="70" t="s">
         <v>193</v>
       </c>
@@ -14720,7 +14721,7 @@
       </c>
     </row>
     <row r="8" spans="1:13" ht="66" customHeight="1">
-      <c r="A8" s="403"/>
+      <c r="A8" s="395"/>
       <c r="B8" s="70" t="s">
         <v>471</v>
       </c>
@@ -14734,10 +14735,10 @@
         <f t="shared" si="1"/>
         <v>540</v>
       </c>
-      <c r="F8" s="405"/>
-      <c r="G8" s="405"/>
+      <c r="F8" s="406"/>
+      <c r="G8" s="406"/>
       <c r="H8" s="346"/>
-      <c r="I8" s="403"/>
+      <c r="I8" s="395"/>
       <c r="J8" s="70" t="s">
         <v>194</v>
       </c>
@@ -14752,7 +14753,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="57" customHeight="1">
-      <c r="A9" s="403"/>
+      <c r="A9" s="395"/>
       <c r="B9" s="70" t="s">
         <v>194</v>
       </c>
@@ -14766,10 +14767,10 @@
         <f t="shared" si="1"/>
         <v>320</v>
       </c>
-      <c r="F9" s="405"/>
-      <c r="G9" s="405"/>
+      <c r="F9" s="406"/>
+      <c r="G9" s="406"/>
       <c r="H9" s="346"/>
-      <c r="I9" s="402" t="s">
+      <c r="I9" s="394" t="s">
         <v>195</v>
       </c>
       <c r="J9" s="189" t="s">
@@ -14807,7 +14808,7 @@
       <c r="F10" s="283"/>
       <c r="G10" s="283"/>
       <c r="H10" s="346"/>
-      <c r="I10" s="403"/>
+      <c r="I10" s="395"/>
       <c r="J10" s="189" t="s">
         <v>197</v>
       </c>
@@ -14841,7 +14842,7 @@
       <c r="F11" s="190"/>
       <c r="G11" s="190"/>
       <c r="H11" s="346"/>
-      <c r="I11" s="406"/>
+      <c r="I11" s="396"/>
       <c r="J11" s="294" t="s">
         <v>198</v>
       </c>
@@ -14926,7 +14927,7 @@
       </c>
     </row>
     <row r="14" spans="1:13" ht="28">
-      <c r="A14" s="394" t="s">
+      <c r="A14" s="397" t="s">
         <v>204</v>
       </c>
       <c r="B14" s="286" t="s">
@@ -14945,7 +14946,7 @@
       <c r="F14" s="76"/>
       <c r="G14" s="41"/>
       <c r="H14" s="41"/>
-      <c r="I14" s="394" t="s">
+      <c r="I14" s="397" t="s">
         <v>204</v>
       </c>
       <c r="J14" s="286" t="s">
@@ -14962,7 +14963,7 @@
       </c>
     </row>
     <row r="15" spans="1:13" ht="28">
-      <c r="A15" s="395"/>
+      <c r="A15" s="398"/>
       <c r="B15" s="289" t="s">
         <v>589</v>
       </c>
@@ -14979,7 +14980,7 @@
       <c r="F15" s="78"/>
       <c r="G15" s="43"/>
       <c r="H15" s="43"/>
-      <c r="I15" s="395"/>
+      <c r="I15" s="398"/>
       <c r="J15" s="289" t="s">
         <v>206</v>
       </c>
@@ -14994,7 +14995,7 @@
       </c>
     </row>
     <row r="16" spans="1:13" ht="28">
-      <c r="A16" s="395"/>
+      <c r="A16" s="398"/>
       <c r="B16" s="289" t="s">
         <v>590</v>
       </c>
@@ -15011,7 +15012,7 @@
       <c r="F16" s="78"/>
       <c r="G16" s="43"/>
       <c r="H16" s="43"/>
-      <c r="I16" s="395"/>
+      <c r="I16" s="398"/>
       <c r="J16" s="289" t="s">
         <v>207</v>
       </c>
@@ -15026,7 +15027,7 @@
       </c>
     </row>
     <row r="17" spans="1:13" ht="28">
-      <c r="A17" s="395"/>
+      <c r="A17" s="398"/>
       <c r="B17" s="289" t="s">
         <v>591</v>
       </c>
@@ -15043,7 +15044,7 @@
       <c r="F17" s="78"/>
       <c r="G17" s="43"/>
       <c r="H17" s="43"/>
-      <c r="I17" s="395"/>
+      <c r="I17" s="398"/>
       <c r="J17" s="289" t="s">
         <v>208</v>
       </c>
@@ -15059,7 +15060,7 @@
       </c>
     </row>
     <row r="18" spans="1:13">
-      <c r="A18" s="395"/>
+      <c r="A18" s="398"/>
       <c r="B18" s="293" t="s">
         <v>209</v>
       </c>
@@ -15076,7 +15077,7 @@
       <c r="F18" s="78"/>
       <c r="G18" s="43"/>
       <c r="H18" s="43"/>
-      <c r="I18" s="395"/>
+      <c r="I18" s="398"/>
       <c r="J18" s="293" t="s">
         <v>209</v>
       </c>
@@ -15091,7 +15092,7 @@
       </c>
     </row>
     <row r="19" spans="1:13" ht="31.5" customHeight="1">
-      <c r="A19" s="395"/>
+      <c r="A19" s="398"/>
       <c r="B19" s="195" t="s">
         <v>210</v>
       </c>
@@ -15110,7 +15111,7 @@
       </c>
       <c r="G19" s="43"/>
       <c r="H19" s="43"/>
-      <c r="I19" s="395"/>
+      <c r="I19" s="398"/>
       <c r="J19" s="195" t="s">
         <v>210</v>
       </c>
@@ -15126,7 +15127,7 @@
       </c>
     </row>
     <row r="20" spans="1:13" ht="28">
-      <c r="A20" s="396"/>
+      <c r="A20" s="399"/>
       <c r="B20" s="70"/>
       <c r="C20" s="186"/>
       <c r="D20" s="82"/>
@@ -15134,7 +15135,7 @@
       <c r="F20" s="44"/>
       <c r="G20" s="44"/>
       <c r="H20" s="44"/>
-      <c r="I20" s="396"/>
+      <c r="I20" s="399"/>
       <c r="J20" s="372" t="s">
         <v>212</v>
       </c>
@@ -15176,12 +15177,12 @@
       </c>
     </row>
     <row r="22" spans="1:13" ht="27" customHeight="1">
-      <c r="A22" s="397" t="s">
+      <c r="A22" s="400" t="s">
         <v>215</v>
       </c>
-      <c r="B22" s="398"/>
-      <c r="C22" s="398"/>
-      <c r="D22" s="399"/>
+      <c r="B22" s="401"/>
+      <c r="C22" s="401"/>
+      <c r="D22" s="402"/>
       <c r="E22" s="196">
         <f>SUM(E4:E21)</f>
         <v>60260</v>
@@ -15189,24 +15190,24 @@
       <c r="F22" s="47"/>
       <c r="G22" s="48"/>
       <c r="H22" s="370"/>
-      <c r="I22" s="397" t="s">
+      <c r="I22" s="400" t="s">
         <v>215</v>
       </c>
-      <c r="J22" s="398"/>
-      <c r="K22" s="398"/>
-      <c r="L22" s="399"/>
+      <c r="J22" s="401"/>
+      <c r="K22" s="401"/>
+      <c r="L22" s="402"/>
       <c r="M22" s="196">
         <f>SUM(M4:M21)</f>
         <v>50895</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="27" customHeight="1">
-      <c r="A23" s="397" t="s">
+      <c r="A23" s="400" t="s">
         <v>216</v>
       </c>
-      <c r="B23" s="398"/>
-      <c r="C23" s="398"/>
-      <c r="D23" s="399"/>
+      <c r="B23" s="401"/>
+      <c r="C23" s="401"/>
+      <c r="D23" s="402"/>
       <c r="E23" s="196">
         <f>'DS khách mời dự tính 2025'!G79</f>
         <v>68800</v>
@@ -15214,12 +15215,12 @@
       <c r="F23" s="47"/>
       <c r="G23" s="48"/>
       <c r="H23" s="370"/>
-      <c r="I23" s="397" t="s">
+      <c r="I23" s="400" t="s">
         <v>216</v>
       </c>
-      <c r="J23" s="398"/>
-      <c r="K23" s="398"/>
-      <c r="L23" s="399"/>
+      <c r="J23" s="401"/>
+      <c r="K23" s="401"/>
+      <c r="L23" s="402"/>
       <c r="M23" s="196">
         <f>'DS khách mời dự tính 2024'!O79</f>
         <v>0</v>
@@ -15248,11 +15249,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="I4:I8"/>
-    <mergeCell ref="I9:I11"/>
-    <mergeCell ref="I14:I20"/>
-    <mergeCell ref="I22:L22"/>
-    <mergeCell ref="I23:L23"/>
     <mergeCell ref="A14:A20"/>
     <mergeCell ref="A22:D22"/>
     <mergeCell ref="A23:D23"/>
@@ -15262,6 +15258,11 @@
     <mergeCell ref="F4:F6"/>
     <mergeCell ref="G4:G9"/>
     <mergeCell ref="F7:F9"/>
+    <mergeCell ref="I4:I8"/>
+    <mergeCell ref="I9:I11"/>
+    <mergeCell ref="I14:I20"/>
+    <mergeCell ref="I22:L22"/>
+    <mergeCell ref="I23:L23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="40" orientation="landscape" r:id="rId1"/>
@@ -15272,10 +15273,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40863F83-52D9-4C43-B2FD-270942BBA802}">
   <dimension ref="B1:N82"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageBreakPreview" topLeftCell="B1" zoomScale="85" zoomScaleNormal="115" zoomScaleSheetLayoutView="85" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="B1" zoomScale="85" zoomScaleNormal="115" zoomScaleSheetLayoutView="85" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="M11" sqref="M11"/>
-      <selection pane="bottomLeft" activeCell="B59" sqref="B59:B77"/>
+      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>

</xml_diff>